<commit_message>
experiments run 16 September
</commit_message>
<xml_diff>
--- a/results/I2_N10_T100_C200_0_mean_res.xlsx
+++ b/results/I2_N10_T100_C200_0_mean_res.xlsx
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3600.063000202179</v>
+        <v>43200.26300001144</v>
       </c>
     </row>
     <row r="5">
@@ -493,7 +493,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9942929473789498</v>
+        <v>0.9890717578741405</v>
       </c>
     </row>
     <row r="6">

</xml_diff>